<commit_message>
Added comments to the game back-end. Separated the work in diferent modules (clases) and methods.
</commit_message>
<xml_diff>
--- a/1Homework/DataBase/diamond.xlsx
+++ b/1Homework/DataBase/diamond.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R1e17dad6698c466a"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R52e5f7d6098a4f4b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -36,8 +36,8 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FF1DCBD7"/>
-        <x:bgColor rgb="FF1DCBD7"/>
+        <x:fgColor rgb="FF4064F2"/>
+        <x:bgColor rgb="FF4064F2"/>
       </x:patternFill>
     </x:fill>
   </x:fills>

</xml_diff>